<commit_message>
2000 and 2010 Census added
</commit_message>
<xml_diff>
--- a/data/ECvotes.xlsx
+++ b/data/ECvotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LK296/Documents/Research/Electoral College Distortion/EC-Analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leekennedyshaffer/Documents/Research/Electoral College Distortion/EC-Analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3113EF47-72F9-2B44-9415-C3024F2B701B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A150D7E-74FA-464B-B62F-9E0D3B982B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{F3862A4C-2B2E-8747-A0F5-1103E047C4F6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16680" xr2:uid="{F3862A4C-2B2E-8747-A0F5-1103E047C4F6}"/>
   </bookViews>
   <sheets>
     <sheet name="EC" sheetId="3" r:id="rId1"/>
@@ -189,25 +189,25 @@
     <t>WY</t>
   </si>
   <si>
-    <t>ME-1</t>
-  </si>
-  <si>
-    <t>ME-2</t>
-  </si>
-  <si>
     <t>DC</t>
   </si>
   <si>
-    <t>NE-1</t>
-  </si>
-  <si>
-    <t>NE-2</t>
-  </si>
-  <si>
-    <t>NE-3</t>
-  </si>
-  <si>
     <t>PR</t>
+  </si>
+  <si>
+    <t>ME01</t>
+  </si>
+  <si>
+    <t>ME02</t>
+  </si>
+  <si>
+    <t>NE01</t>
+  </si>
+  <si>
+    <t>NE02</t>
+  </si>
+  <si>
+    <t>NE03</t>
   </si>
 </sst>
 </file>
@@ -579,10 +579,10 @@
   <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A59" sqref="A59"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" s="2">
         <v>3</v>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B32" s="2">
         <v>0</v>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2">
         <v>0</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B34" s="2">
         <v>0</v>
@@ -3623,7 +3623,7 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B58" s="2">
         <v>0</v>

</xml_diff>